<commit_message>
Work on activating sheets/cells.
</commit_message>
<xml_diff>
--- a/examples/ranges/template.xlsx
+++ b/examples/ranges/template.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djohnson\Code\GitHub\xlsx-populate\examples\ranges\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="7755" windowWidth="15360" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ClickThroughRateSheet" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="ClickThroughRateSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName localSheetId="0" name="ALL_CLK">OFFSET(ClickThroughRateSheet!$B$3,0,0,COUNTA(ClickThroughRateSheet!$B:$B)-1)</definedName>
-    <definedName localSheetId="0" name="All_CTR">OFFSET(ClickThroughRateSheet!$D$3,0,0,COUNTA(ClickThroughRateSheet!$D:$D)-1)</definedName>
-    <definedName localSheetId="0" name="ALL_IMP">OFFSET(ClickThroughRateSheet!$C$3,0,0,COUNTA(ClickThroughRateSheet!$C:$C)-1)</definedName>
+    <definedName name="ALL_CLK" localSheetId="0">OFFSET(ClickThroughRateSheet!$B$3,0,0,COUNTA(ClickThroughRateSheet!$B:$B)-1)</definedName>
+    <definedName name="All_CTR" localSheetId="0">OFFSET(ClickThroughRateSheet!$D$3,0,0,COUNTA(ClickThroughRateSheet!$D:$D)-1)</definedName>
+    <definedName name="ALL_IMP" localSheetId="0">OFFSET(ClickThroughRateSheet!$C$3,0,0,COUNTA(ClickThroughRateSheet!$C:$C)-1)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
@@ -109,7 +110,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -153,7 +154,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -238,6 +238,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4091-4A73-8AC4-DE63EE05161B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -324,6 +329,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4091-4A73-8AC4-DE63EE05161B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -371,7 +381,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -491,7 +500,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -589,7 +597,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -681,7 +688,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1308,7 +1314,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1402,6 +1414,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1437,6 +1466,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1588,17 +1634,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="11.7109375"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="12"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1623,7 +1669,8 @@
         <v>398503</v>
       </c>
       <c r="D3" s="4">
-        <f ref="D3:D7" si="0" t="shared">B3/C3</f>
+        <f t="shared" ref="D3:D7" si="0">B3/C3</f>
+        <v>1.0614725610597661E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1634,7 +1681,8 @@
         <v>460983</v>
       </c>
       <c r="D4" s="4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
+        <v>1.6421429857500169E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1645,7 +1693,8 @@
         <v>342456</v>
       </c>
       <c r="D5" s="4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
+        <v>6.8621954353259985E-4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1656,7 +1705,8 @@
         <v>235098</v>
       </c>
       <c r="D6" s="4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
+        <v>6.1676407285472443E-4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1667,7 +1717,8 @@
         <v>53843</v>
       </c>
       <c r="D7" s="4">
-        <f si="0" t="shared"/>
+        <f t="shared" si="0"/>
+        <v>2.4887171962929256E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1678,20 +1729,34 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>